<commit_message>
Custom risk thresholds updated
</commit_message>
<xml_diff>
--- a/dist/risk_threshold.xlsx
+++ b/dist/risk_threshold.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsalo\PhpstormProjects\wiat_front\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25683F59-CEA7-4536-8D9B-A635493C6896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A09C6433-024A-4EEA-8538-18A0CA4DC5E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{C8DB30FF-034D-4F5E-A8CE-87B2AA9556C4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Low</t>
   </si>
@@ -100,7 +100,53 @@
   </si>
   <si>
     <r>
-      <t>Toxic units in the effluent</t>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> --&gt; Higher values means higher impacts</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> --&gt; Higher values means lower impacts</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Increase of the concentration of the pollutants in the receiving water body after discharge (with respect to EQS)</t>
     </r>
     <r>
       <rPr>
@@ -118,6 +164,18 @@
   <si>
     <r>
       <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Eutrophication potential</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <vertAlign val="superscript"/>
         <sz val="11"/>
         <color theme="1"/>
@@ -127,43 +185,10 @@
       </rPr>
       <t>1</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> --&gt; Higher values means higher impacts</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> --&gt; Higher values means lower impacts</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>GHG emissions from Wastewater</t>
+  </si>
+  <si>
+    <r>
+      <t>Increase in temperature in the receiving water body due to industry discharge</t>
     </r>
     <r>
       <rPr>
@@ -180,66 +205,7 @@
   </si>
   <si>
     <r>
-      <t>Increase of the concentration of the pollutants in the receiving water body after discharge (with respect to EQS)</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Eutrophication potential</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Concentration of the pollutants in the effluent (with respect to EQS)</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Carbon impact</t>
+      <t>GHG emissions from wastewater treatment</t>
     </r>
     <r>
       <rPr>
@@ -348,7 +314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -358,7 +324,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -676,15 +641,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{131E30A0-4211-4C5A-8B5B-19CA9E80E21E}">
-  <dimension ref="A3:F22"/>
+  <dimension ref="A3:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="66.1796875" customWidth="1"/>
+    <col min="1" max="1" width="67.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -702,45 +667,45 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:6" ht="31" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -748,8 +713,8 @@
       <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
-        <v>13</v>
+      <c r="A9" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -757,47 +722,25 @@
       <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>4</v>
+      <c r="A10" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="16" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+    <row r="14" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" s="5"/>
-    </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>